<commit_message>
notes, thesis and DP-GBDT
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>SCHEDULE START TIME</t>
   </si>
@@ -91,6 +91,24 @@
   <si>
     <t>SUN</t>
   </si>
+  <si>
+    <t>Read, Read, Read</t>
+  </si>
+  <si>
+    <t>watch videos on GB and GBDT math, make notes</t>
+  </si>
+  <si>
+    <t>setup new printer for papers</t>
+  </si>
+  <si>
+    <t>setup time log</t>
+  </si>
+  <si>
+    <t>read DP-GBDT paper &amp; theos thesis</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
@@ -99,13 +117,13 @@
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="h:mm\ AM/PM"/>
     <numFmt numFmtId="177" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
-    <numFmt numFmtId="178" formatCode="[$-409]h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="31">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -172,18 +190,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9.75"/>
+      <color rgb="FF242729"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9.75"/>
+      <color theme="1"/>
+      <name val="Liberation Mono"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="0"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Century Gothic"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -191,6 +213,36 @@
       <color rgb="FFFFFFFF"/>
       <name val="Century Gothic"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Century Gothic"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Century Gothic"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Century Gothic"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -204,17 +256,31 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Century Gothic"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Century Gothic"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F76"/>
       <name val="Century Gothic"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Century Gothic"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -227,7 +293,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Century Gothic"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -235,12 +301,20 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Century Gothic"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Century Gothic"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
@@ -263,48 +337,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Century Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Century Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Century Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Century Gothic"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Century Gothic"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Century Gothic"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -314,15 +351,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Century Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="44">
+  <fills count="46">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,49 +361,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.15"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.0499893185216834"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.149998474074526"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.15"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.0499893185216834"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.149998474074526"/>
+        <fgColor theme="4" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,25 +445,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,25 +553,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,7 +595,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,114 +619,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -663,6 +705,17 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -674,6 +727,24 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -737,24 +808,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -763,150 +816,150 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="42" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="41" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="43" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="10" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="43" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="44" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="42" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="41" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="45" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="39" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="40" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="13" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="9" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="12" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="11" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="11" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
@@ -952,6 +1005,33 @@
     <xf numFmtId="178" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="178" fontId="7" fillId="10" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="10" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="11" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="11" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="11" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="10" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="10" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="10" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="10" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -961,20 +1041,30 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="10" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="177" fontId="6" fillId="12" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
@@ -1320,271 +1410,271 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="2.85833333333333" customWidth="true"/>
-    <col min="2" max="2" width="14.425" style="22" customWidth="true"/>
+    <col min="2" max="2" width="14.425" style="35" customWidth="true"/>
     <col min="3" max="3" width="3.28333333333333" customWidth="true"/>
     <col min="5" max="5" width="2.425" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="23"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="A1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" ht="38" customHeight="true" spans="1:5">
-      <c r="A2" s="23"/>
-      <c r="B2" s="25" t="s">
+      <c r="A2" s="36"/>
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="25" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="23"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="23"/>
-      <c r="B3" s="26">
+      <c r="A3" s="36"/>
+      <c r="B3" s="39">
         <v>0.25</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="26" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="23"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="23"/>
-      <c r="B4" s="26">
+      <c r="A4" s="36"/>
+      <c r="B4" s="39">
         <v>0.291666666666667</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="26" t="s">
+      <c r="C4" s="36"/>
+      <c r="D4" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="23"/>
-      <c r="B5" s="26">
+      <c r="A5" s="36"/>
+      <c r="B5" s="39">
         <v>0.333333333333333</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="26" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="36"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="23"/>
-      <c r="B6" s="26">
+      <c r="A6" s="36"/>
+      <c r="B6" s="39">
         <v>0.375</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="26" t="s">
+      <c r="C6" s="36"/>
+      <c r="D6" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="36"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="23"/>
-      <c r="B7" s="26">
+      <c r="A7" s="36"/>
+      <c r="B7" s="39">
         <v>0.416666666666667</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="26" t="s">
+      <c r="C7" s="36"/>
+      <c r="D7" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="36"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="23"/>
-      <c r="B8" s="26">
+      <c r="A8" s="36"/>
+      <c r="B8" s="39">
         <v>0.458333333333333</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="26" t="s">
+      <c r="C8" s="36"/>
+      <c r="D8" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="23"/>
+      <c r="E8" s="36"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="23"/>
-      <c r="B9" s="26">
+      <c r="A9" s="36"/>
+      <c r="B9" s="39">
         <v>0.5</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="27" t="s">
+      <c r="C9" s="36"/>
+      <c r="D9" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="23"/>
+      <c r="E9" s="36"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="23"/>
-      <c r="B10" s="26">
+      <c r="A10" s="36"/>
+      <c r="B10" s="39">
         <v>0.541666666666667</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="27" t="s">
+      <c r="C10" s="36"/>
+      <c r="D10" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="23"/>
+      <c r="E10" s="36"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="23"/>
-      <c r="B11" s="26">
+      <c r="A11" s="36"/>
+      <c r="B11" s="39">
         <v>0.583333333333333</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="27" t="s">
+      <c r="C11" s="36"/>
+      <c r="D11" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
+      <c r="E11" s="36"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="23"/>
-      <c r="B12" s="26">
+      <c r="A12" s="36"/>
+      <c r="B12" s="39">
         <v>0.625</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="27" t="s">
+      <c r="C12" s="36"/>
+      <c r="D12" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="23"/>
+      <c r="E12" s="36"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="23"/>
-      <c r="B13" s="26">
+      <c r="A13" s="36"/>
+      <c r="B13" s="39">
         <v>0.666666666666667</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="23"/>
-      <c r="B14" s="26">
+      <c r="A14" s="36"/>
+      <c r="B14" s="39">
         <v>0.708333333333333</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="23"/>
-      <c r="B15" s="26">
+      <c r="A15" s="36"/>
+      <c r="B15" s="39">
         <v>0.75</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="23"/>
-      <c r="B16" s="26">
+      <c r="A16" s="36"/>
+      <c r="B16" s="39">
         <v>0.791666666666667</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="23"/>
-      <c r="B17" s="26">
+      <c r="A17" s="36"/>
+      <c r="B17" s="39">
         <v>0.833333333333333</v>
       </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="23"/>
-      <c r="B18" s="26">
+      <c r="A18" s="36"/>
+      <c r="B18" s="39">
         <v>0.875</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="23"/>
-      <c r="B19" s="26">
+      <c r="A19" s="36"/>
+      <c r="B19" s="39">
         <v>0.916666666666667</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="23"/>
-      <c r="B20" s="26">
+      <c r="A20" s="36"/>
+      <c r="B20" s="39">
         <v>0.958333333333333</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="23"/>
-      <c r="B21" s="26">
+      <c r="A21" s="36"/>
+      <c r="B21" s="39">
         <v>0</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="23"/>
-      <c r="B22" s="26">
+      <c r="A22" s="36"/>
+      <c r="B22" s="39">
         <v>0.0416666666666667</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="23"/>
-      <c r="B23" s="26">
+      <c r="A23" s="36"/>
+      <c r="B23" s="39">
         <v>0.0833333333333333</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="23"/>
-      <c r="B24" s="26">
+      <c r="A24" s="36"/>
+      <c r="B24" s="39">
         <v>0.125</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="23"/>
-      <c r="B25" s="26">
+      <c r="A25" s="36"/>
+      <c r="B25" s="39">
         <v>0.166666666666667</v>
       </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="23"/>
-      <c r="B26" s="26">
+      <c r="A26" s="36"/>
+      <c r="B26" s="39">
         <v>0.208333333333333</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="23"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1612,7 +1702,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:2">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="34" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1639,13 +1729,13 @@
       <c r="D8" s="6">
         <v>0.291666666666667</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="27">
         <v>44319</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="28">
         <f>--LEFT(E8,3)</f>
         <v>15</v>
       </c>
@@ -1669,10 +1759,10 @@
       <c r="F9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="29" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1698,11 +1788,11 @@
         <f t="shared" si="0"/>
         <v>44323</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="30">
         <f t="shared" si="0"/>
         <v>44324</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="30">
         <f t="shared" si="0"/>
         <v>44325</v>
       </c>
@@ -2580,8 +2670,8 @@
   <sheetPr/>
   <dimension ref="A2:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -2593,9 +2683,12 @@
     <col min="11" max="16384" width="10.7083333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" s="1" customFormat="true" spans="2:2">
+    <row r="2" s="1" customFormat="true" spans="2:3">
       <c r="B2" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="true" ht="18" customHeight="true" spans="1:6">
@@ -2621,13 +2714,13 @@
       <c r="D8" s="6">
         <v>0.291666666666667</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="27">
         <v>44319</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="28">
         <f>--LEFT(E8,3)</f>
         <v>15</v>
       </c>
@@ -2651,10 +2744,10 @@
       <c r="F9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="29" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2680,16 +2773,16 @@
         <f t="shared" si="0"/>
         <v>44323</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="30">
         <f t="shared" si="0"/>
         <v>44324</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="30">
         <f t="shared" si="0"/>
         <v>44325</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="11" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A11" s="15">
         <f>D8</f>
         <v>0.291666666666667</v>
@@ -2702,7 +2795,7 @@
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
     </row>
-    <row r="12" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="12" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A12" s="16">
         <f>A11+TIME(0,myinterval,0)</f>
         <v>0.302083333333333</v>
@@ -2715,7 +2808,7 @@
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
     </row>
-    <row r="13" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="13" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A13" s="15">
         <f>A12+TIME(0,myinterval,0)</f>
         <v>0.3125</v>
@@ -2728,7 +2821,7 @@
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
     </row>
-    <row r="14" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="14" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A14" s="16">
         <f>A13+TIME(0,myinterval,0)</f>
         <v>0.322916666666667</v>
@@ -2741,12 +2834,14 @@
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
     </row>
-    <row r="15" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="15" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A15" s="15">
         <f>A14+TIME(0,myinterval,0)</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="B15" s="15"/>
+      <c r="B15" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
@@ -2754,12 +2849,12 @@
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
     </row>
-    <row r="16" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="16" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A16" s="16">
         <f>A15+TIME(0,myinterval,0)</f>
         <v>0.34375</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
@@ -2767,12 +2862,12 @@
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
     </row>
-    <row r="17" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="17" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A17" s="15">
         <f>A16+TIME(0,myinterval,0)</f>
         <v>0.354166666666667</v>
       </c>
-      <c r="B17" s="15"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
@@ -2780,12 +2875,12 @@
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
     </row>
-    <row r="18" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="18" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A18" s="16">
         <f>A17+TIME(0,myinterval,0)</f>
         <v>0.364583333333333</v>
       </c>
-      <c r="B18" s="16"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
@@ -2793,12 +2888,12 @@
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
     </row>
-    <row r="19" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="19" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A19" s="15">
         <f>A18+TIME(0,myinterval,0)</f>
         <v>0.375</v>
       </c>
-      <c r="B19" s="15"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
@@ -2806,12 +2901,12 @@
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
     </row>
-    <row r="20" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="20" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A20" s="16">
         <f>A19+TIME(0,myinterval,0)</f>
         <v>0.385416666666667</v>
       </c>
-      <c r="B20" s="16"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
@@ -2819,12 +2914,12 @@
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
     </row>
-    <row r="21" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="21" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A21" s="15">
         <f>A20+TIME(0,myinterval,0)</f>
         <v>0.395833333333334</v>
       </c>
-      <c r="B21" s="15"/>
+      <c r="B21" s="18"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
@@ -2832,7 +2927,7 @@
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
     </row>
-    <row r="22" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="22" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A22" s="16">
         <f>A21+TIME(0,myinterval,0)</f>
         <v>0.40625</v>
@@ -2845,12 +2940,14 @@
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
     </row>
-    <row r="23" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="23" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A23" s="15">
         <f>A22+TIME(0,myinterval,0)</f>
         <v>0.416666666666667</v>
       </c>
-      <c r="B23" s="15"/>
+      <c r="B23" s="19" t="s">
+        <v>25</v>
+      </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
@@ -2858,12 +2955,12 @@
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
     </row>
-    <row r="24" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="24" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A24" s="16">
         <f>A23+TIME(0,myinterval,0)</f>
         <v>0.427083333333334</v>
       </c>
-      <c r="B24" s="16"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
@@ -2871,12 +2968,12 @@
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
     </row>
-    <row r="25" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="25" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A25" s="15">
         <f>A24+TIME(0,myinterval,0)</f>
         <v>0.4375</v>
       </c>
-      <c r="B25" s="15"/>
+      <c r="B25" s="20"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
@@ -2884,12 +2981,12 @@
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
     </row>
-    <row r="26" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="26" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A26" s="16">
         <f>A25+TIME(0,myinterval,0)</f>
         <v>0.447916666666667</v>
       </c>
-      <c r="B26" s="16"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
@@ -2897,12 +2994,12 @@
       <c r="G26" s="16"/>
       <c r="H26" s="16"/>
     </row>
-    <row r="27" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="27" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A27" s="15">
         <f>A26+TIME(0,myinterval,0)</f>
         <v>0.458333333333334</v>
       </c>
-      <c r="B27" s="15"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
@@ -2910,12 +3007,14 @@
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
     </row>
-    <row r="28" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="28" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A28" s="16">
         <f>A27+TIME(0,myinterval,0)</f>
         <v>0.46875</v>
       </c>
-      <c r="B28" s="16"/>
+      <c r="B28" s="19" t="s">
+        <v>26</v>
+      </c>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -2923,12 +3022,12 @@
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
     </row>
-    <row r="29" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="29" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A29" s="15">
         <f>A28+TIME(0,myinterval,0)</f>
         <v>0.479166666666667</v>
       </c>
-      <c r="B29" s="15"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
@@ -2936,12 +3035,14 @@
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
     </row>
-    <row r="30" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="30" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A30" s="16">
         <f>A29+TIME(0,myinterval,0)</f>
         <v>0.489583333333334</v>
       </c>
-      <c r="B30" s="16"/>
+      <c r="B30" s="17" t="s">
+        <v>27</v>
+      </c>
       <c r="C30" s="16"/>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
@@ -2949,12 +3050,12 @@
       <c r="G30" s="16"/>
       <c r="H30" s="16"/>
     </row>
-    <row r="31" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="31" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A31" s="15">
         <f>A30+TIME(0,myinterval,0)</f>
         <v>0.5</v>
       </c>
-      <c r="B31" s="15"/>
+      <c r="B31" s="18"/>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
@@ -2962,12 +3063,12 @@
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
     </row>
-    <row r="32" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="32" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A32" s="16">
         <f>A31+TIME(0,myinterval,0)</f>
         <v>0.510416666666667</v>
       </c>
-      <c r="B32" s="16"/>
+      <c r="B32" s="18"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
@@ -2975,12 +3076,12 @@
       <c r="G32" s="16"/>
       <c r="H32" s="16"/>
     </row>
-    <row r="33" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="33" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A33" s="15">
         <f>A32+TIME(0,myinterval,0)</f>
         <v>0.520833333333334</v>
       </c>
-      <c r="B33" s="15"/>
+      <c r="B33" s="22"/>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
@@ -2988,7 +3089,7 @@
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
     </row>
-    <row r="34" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="34" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A34" s="16">
         <f>A33+TIME(0,myinterval,0)</f>
         <v>0.53125</v>
@@ -3000,7 +3101,7 @@
       <c r="G34" s="16"/>
       <c r="H34" s="16"/>
     </row>
-    <row r="35" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="35" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A35" s="15">
         <f>A34+TIME(0,myinterval,0)</f>
         <v>0.541666666666667</v>
@@ -3013,7 +3114,7 @@
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
     </row>
-    <row r="36" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="36" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A36" s="16">
         <f>A35+TIME(0,myinterval,0)</f>
         <v>0.552083333333333</v>
@@ -3026,12 +3127,14 @@
       <c r="G36" s="16"/>
       <c r="H36" s="16"/>
     </row>
-    <row r="37" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="37" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A37" s="15">
         <f>A36+TIME(0,myinterval,0)</f>
         <v>0.5625</v>
       </c>
-      <c r="B37" s="15"/>
+      <c r="B37" s="17" t="s">
+        <v>27</v>
+      </c>
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
@@ -3039,12 +3142,12 @@
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
     </row>
-    <row r="38" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="38" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A38" s="16">
         <f>A37+TIME(0,myinterval,0)</f>
         <v>0.572916666666667</v>
       </c>
-      <c r="B38" s="16"/>
+      <c r="B38" s="18"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
@@ -3052,12 +3155,12 @@
       <c r="G38" s="16"/>
       <c r="H38" s="16"/>
     </row>
-    <row r="39" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="39" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A39" s="15">
         <f>A38+TIME(0,myinterval,0)</f>
         <v>0.583333333333333</v>
       </c>
-      <c r="B39" s="15"/>
+      <c r="B39" s="18"/>
       <c r="C39" s="15"/>
       <c r="D39" s="15"/>
       <c r="E39" s="15"/>
@@ -3065,12 +3168,12 @@
       <c r="G39" s="15"/>
       <c r="H39" s="15"/>
     </row>
-    <row r="40" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="40" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A40" s="16">
         <f>A39+TIME(0,myinterval,0)</f>
         <v>0.59375</v>
       </c>
-      <c r="B40" s="16"/>
+      <c r="B40" s="18"/>
       <c r="C40" s="16"/>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
@@ -3078,12 +3181,12 @@
       <c r="G40" s="16"/>
       <c r="H40" s="16"/>
     </row>
-    <row r="41" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="41" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A41" s="15">
         <f>A40+TIME(0,myinterval,0)</f>
         <v>0.604166666666667</v>
       </c>
-      <c r="B41" s="15"/>
+      <c r="B41" s="22"/>
       <c r="C41" s="15"/>
       <c r="D41" s="15"/>
       <c r="E41" s="15"/>
@@ -3091,7 +3194,7 @@
       <c r="G41" s="15"/>
       <c r="H41" s="15"/>
     </row>
-    <row r="42" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="42" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A42" s="16">
         <f>A41+TIME(0,myinterval,0)</f>
         <v>0.614583333333333</v>
@@ -3104,12 +3207,14 @@
       <c r="G42" s="16"/>
       <c r="H42" s="16"/>
     </row>
-    <row r="43" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="43" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A43" s="15">
         <f>A42+TIME(0,myinterval,0)</f>
         <v>0.625</v>
       </c>
-      <c r="B43" s="15"/>
+      <c r="B43" s="23" t="s">
+        <v>27</v>
+      </c>
       <c r="C43" s="15"/>
       <c r="D43" s="15"/>
       <c r="E43" s="15"/>
@@ -3117,12 +3222,12 @@
       <c r="G43" s="15"/>
       <c r="H43" s="15"/>
     </row>
-    <row r="44" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="44" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A44" s="16">
         <f>A43+TIME(0,myinterval,0)</f>
         <v>0.635416666666667</v>
       </c>
-      <c r="B44" s="16"/>
+      <c r="B44" s="24"/>
       <c r="C44" s="16"/>
       <c r="D44" s="16"/>
       <c r="E44" s="16"/>
@@ -3130,12 +3235,12 @@
       <c r="G44" s="16"/>
       <c r="H44" s="16"/>
     </row>
-    <row r="45" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="45" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A45" s="15">
         <f>A44+TIME(0,myinterval,0)</f>
         <v>0.645833333333333</v>
       </c>
-      <c r="B45" s="15"/>
+      <c r="B45" s="24"/>
       <c r="C45" s="15"/>
       <c r="D45" s="15"/>
       <c r="E45" s="15"/>
@@ -3143,12 +3248,12 @@
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
     </row>
-    <row r="46" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="46" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A46" s="16">
         <f>A45+TIME(0,myinterval,0)</f>
         <v>0.65625</v>
       </c>
-      <c r="B46" s="16"/>
+      <c r="B46" s="25"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
@@ -3156,7 +3261,7 @@
       <c r="G46" s="16"/>
       <c r="H46" s="16"/>
     </row>
-    <row r="47" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="47" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A47" s="15">
         <f>A46+TIME(0,myinterval,0)</f>
         <v>0.666666666666666</v>
@@ -3169,7 +3274,7 @@
       <c r="G47" s="15"/>
       <c r="H47" s="15"/>
     </row>
-    <row r="48" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="48" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A48" s="16">
         <f>A47+TIME(0,myinterval,0)</f>
         <v>0.677083333333333</v>
@@ -3182,7 +3287,7 @@
       <c r="G48" s="16"/>
       <c r="H48" s="16"/>
     </row>
-    <row r="49" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="49" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A49" s="15">
         <f>A48+TIME(0,myinterval,0)</f>
         <v>0.6875</v>
@@ -3195,7 +3300,7 @@
       <c r="G49" s="15"/>
       <c r="H49" s="15"/>
     </row>
-    <row r="50" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="50" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A50" s="16">
         <f>A49+TIME(0,myinterval,0)</f>
         <v>0.697916666666666</v>
@@ -3208,7 +3313,7 @@
       <c r="G50" s="16"/>
       <c r="H50" s="16"/>
     </row>
-    <row r="51" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="51" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A51" s="15">
         <f>A50+TIME(0,myinterval,0)</f>
         <v>0.708333333333333</v>
@@ -3221,7 +3326,7 @@
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
     </row>
-    <row r="52" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="52" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A52" s="16">
         <f>A51+TIME(0,myinterval,0)</f>
         <v>0.71875</v>
@@ -3234,7 +3339,7 @@
       <c r="G52" s="16"/>
       <c r="H52" s="16"/>
     </row>
-    <row r="53" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="53" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A53" s="15">
         <f>A52+TIME(0,myinterval,0)</f>
         <v>0.729166666666666</v>
@@ -3247,7 +3352,7 @@
       <c r="G53" s="15"/>
       <c r="H53" s="15"/>
     </row>
-    <row r="54" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="54" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A54" s="16">
         <f>A53+TIME(0,myinterval,0)</f>
         <v>0.739583333333333</v>
@@ -3260,7 +3365,7 @@
       <c r="G54" s="16"/>
       <c r="H54" s="16"/>
     </row>
-    <row r="55" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="55" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A55" s="15">
         <f>A54+TIME(0,myinterval,0)</f>
         <v>0.749999999999999</v>
@@ -3273,7 +3378,7 @@
       <c r="G55" s="15"/>
       <c r="H55" s="15"/>
     </row>
-    <row r="56" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="56" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A56" s="16">
         <f>A55+TIME(0,myinterval,0)</f>
         <v>0.760416666666666</v>
@@ -3286,7 +3391,7 @@
       <c r="G56" s="16"/>
       <c r="H56" s="16"/>
     </row>
-    <row r="57" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="57" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A57" s="15">
         <f>A56+TIME(0,myinterval,0)</f>
         <v>0.770833333333333</v>
@@ -3299,7 +3404,7 @@
       <c r="G57" s="15"/>
       <c r="H57" s="15"/>
     </row>
-    <row r="58" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="58" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A58" s="16">
         <f>A57+TIME(0,myinterval,0)</f>
         <v>0.781249999999999</v>
@@ -3312,7 +3417,7 @@
       <c r="G58" s="16"/>
       <c r="H58" s="16"/>
     </row>
-    <row r="59" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="59" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A59" s="15">
         <f>A58+TIME(0,myinterval,0)</f>
         <v>0.791666666666666</v>
@@ -3325,7 +3430,7 @@
       <c r="G59" s="15"/>
       <c r="H59" s="15"/>
     </row>
-    <row r="60" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="60" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A60" s="16">
         <f>A59+TIME(0,myinterval,0)</f>
         <v>0.802083333333333</v>
@@ -3338,7 +3443,7 @@
       <c r="G60" s="16"/>
       <c r="H60" s="16"/>
     </row>
-    <row r="61" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="61" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A61" s="15">
         <f>A60+TIME(0,myinterval,0)</f>
         <v>0.812499999999999</v>
@@ -3351,7 +3456,7 @@
       <c r="G61" s="15"/>
       <c r="H61" s="15"/>
     </row>
-    <row r="62" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="62" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A62" s="16">
         <f>A61+TIME(0,myinterval,0)</f>
         <v>0.822916666666666</v>
@@ -3364,7 +3469,7 @@
       <c r="G62" s="16"/>
       <c r="H62" s="16"/>
     </row>
-    <row r="63" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="63" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A63" s="15">
         <f>A62+TIME(0,myinterval,0)</f>
         <v>0.833333333333332</v>
@@ -3377,7 +3482,7 @@
       <c r="G63" s="15"/>
       <c r="H63" s="15"/>
     </row>
-    <row r="64" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="64" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A64" s="16">
         <f>A63+TIME(0,myinterval,0)</f>
         <v>0.843749999999999</v>
@@ -3390,7 +3495,7 @@
       <c r="G64" s="16"/>
       <c r="H64" s="16"/>
     </row>
-    <row r="65" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="65" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A65" s="15">
         <f>A64+TIME(0,myinterval,0)</f>
         <v>0.854166666666666</v>
@@ -3403,7 +3508,7 @@
       <c r="G65" s="15"/>
       <c r="H65" s="15"/>
     </row>
-    <row r="66" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="66" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A66" s="16">
         <f>A65+TIME(0,myinterval,0)</f>
         <v>0.864583333333332</v>
@@ -3416,7 +3521,7 @@
       <c r="G66" s="16"/>
       <c r="H66" s="16"/>
     </row>
-    <row r="67" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="67" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A67" s="15">
         <f>A66+TIME(0,myinterval,0)</f>
         <v>0.874999999999999</v>
@@ -3429,7 +3534,7 @@
       <c r="G67" s="15"/>
       <c r="H67" s="15"/>
     </row>
-    <row r="68" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="68" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A68" s="16">
         <f>A67+TIME(0,myinterval,0)</f>
         <v>0.885416666666666</v>
@@ -3442,7 +3547,7 @@
       <c r="G68" s="16"/>
       <c r="H68" s="16"/>
     </row>
-    <row r="69" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="69" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A69" s="15">
         <f>A68+TIME(0,myinterval,0)</f>
         <v>0.895833333333332</v>
@@ -3455,7 +3560,7 @@
       <c r="G69" s="15"/>
       <c r="H69" s="15"/>
     </row>
-    <row r="70" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="70" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A70" s="16">
         <f>A69+TIME(0,myinterval,0)</f>
         <v>0.906249999999999</v>
@@ -3468,7 +3573,7 @@
       <c r="G70" s="16"/>
       <c r="H70" s="16"/>
     </row>
-    <row r="71" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="71" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A71" s="15">
         <f>A70+TIME(0,myinterval,0)</f>
         <v>0.916666666666666</v>
@@ -3481,7 +3586,7 @@
       <c r="G71" s="15"/>
       <c r="H71" s="15"/>
     </row>
-    <row r="72" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="72" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A72" s="16">
         <f>A71+TIME(0,myinterval,0)</f>
         <v>0.927083333333332</v>
@@ -3494,7 +3599,7 @@
       <c r="G72" s="16"/>
       <c r="H72" s="16"/>
     </row>
-    <row r="73" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="73" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A73" s="15">
         <f>A72+TIME(0,myinterval,0)</f>
         <v>0.937499999999999</v>
@@ -3507,7 +3612,7 @@
       <c r="G73" s="15"/>
       <c r="H73" s="15"/>
     </row>
-    <row r="74" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="74" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A74" s="16">
         <f>A73+TIME(0,myinterval,0)</f>
         <v>0.947916666666665</v>
@@ -3520,7 +3625,7 @@
       <c r="G74" s="16"/>
       <c r="H74" s="16"/>
     </row>
-    <row r="75" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+    <row r="75" s="1" customFormat="true" ht="17" customHeight="true" spans="1:8">
       <c r="A75" s="15">
         <f>A74+TIME(0,myinterval,0)</f>
         <v>0.958333333333332</v>
@@ -3534,13 +3639,34 @@
       <c r="H75" s="15"/>
     </row>
     <row r="76" customFormat="true" ht="21" customHeight="true"/>
-    <row r="77" customFormat="true" ht="21" customHeight="true"/>
-    <row r="78" customFormat="true" ht="21" customHeight="true"/>
+    <row r="77" customFormat="true" ht="21" customHeight="true" spans="1:2">
+      <c r="A77" t="s">
+        <v>28</v>
+      </c>
+      <c r="B77" s="31">
+        <f>20*15</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="78" customFormat="true" ht="21" customHeight="true" spans="2:2">
+      <c r="B78" s="32" t="str">
+        <f>IF(AND(B77&lt;0,B77&gt;-60),CONCATENATE("-",QUOTIENT(B77,60),":",TEXT(MOD(ABS(B77),60),"00")),CONCATENATE(QUOTIENT(B77,60),":",TEXT(MOD(ABS(B77),60),"00"),"h"))</f>
+        <v>5:00h</v>
+      </c>
+    </row>
     <row r="79" customFormat="true" ht="21" customHeight="true"/>
-    <row r="80" customFormat="true" ht="21" customHeight="true"/>
+    <row r="80" customFormat="true" ht="21" customHeight="true" spans="2:2">
+      <c r="B80" s="33"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="8">
     <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B15:B21"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="B43:B46"/>
     <mergeCell ref="A7:C8"/>
   </mergeCells>
   <dataValidations count="2">

</xml_diff>

<commit_message>
done with theory in thesis
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -2670,8 +2670,8 @@
   <sheetPr/>
   <dimension ref="A2:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="7"/>

</xml_diff>

<commit_message>
more ML notes and questions
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>SCHEDULE START TIME</t>
   </si>
@@ -98,7 +98,13 @@
     <t>watch videos on GB and GBDT math, make notes</t>
   </si>
   <si>
+    <t>Finish theos thesis</t>
+  </si>
+  <si>
     <t>setup new printer for papers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finish DP-GBDT paper, formulate and answer questions </t>
   </si>
   <si>
     <t>setup time log</t>
@@ -115,12 +121,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="177" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="176" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="[$-409]h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="h:mm\ AM/PM"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="31">
@@ -208,39 +214,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Century Gothic"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Century Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Century Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Century Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Century Gothic"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -254,11 +230,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Century Gothic"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -269,9 +245,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Century Gothic"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="3"/>
+      <name val="Century Gothic"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Century Gothic"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -284,6 +275,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Century Gothic"/>
@@ -291,25 +290,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF9C0006"/>
       <name val="Century Gothic"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Century Gothic"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Century Gothic"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Century Gothic"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -323,30 +327,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Century Gothic"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Century Gothic"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Century Gothic"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Century Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Century Gothic"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -445,19 +451,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -469,157 +619,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -731,17 +737,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -750,6 +750,17 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -772,20 +783,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -805,159 +805,165 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="44" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="43" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="39" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="42" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="45" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="41" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="38" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="14" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="44" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="45" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="40" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="42" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="41" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="14" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="11" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="9" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="9" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="12" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="43" borderId="15" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="15" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -972,7 +978,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
@@ -990,46 +996,46 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="6" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="176" fontId="6" fillId="6" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="7" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="176" fontId="6" fillId="7" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="8" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="176" fontId="6" fillId="8" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="9" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="177" fontId="7" fillId="9" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="177" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="10" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="177" fontId="7" fillId="10" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="10" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="177" fontId="7" fillId="10" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="11" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="177" fontId="7" fillId="10" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="11" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="177" fontId="7" fillId="11" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="11" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="177" fontId="7" fillId="11" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="10" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="177" fontId="7" fillId="10" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="10" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="177" fontId="7" fillId="10" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="10" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="177" fontId="7" fillId="11" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="10" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="177" fontId="7" fillId="10" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
@@ -1044,7 +1050,7 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="12" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="176" fontId="6" fillId="12" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
@@ -1067,10 +1073,10 @@
     <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
@@ -2671,7 +2677,7 @@
   <dimension ref="A2:H80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -2868,7 +2874,9 @@
         <v>0.354166666666667</v>
       </c>
       <c r="B17" s="18"/>
-      <c r="C17" s="15"/>
+      <c r="C17" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -2881,7 +2889,7 @@
         <v>0.364583333333333</v>
       </c>
       <c r="B18" s="18"/>
-      <c r="C18" s="16"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
@@ -2894,7 +2902,7 @@
         <v>0.375</v>
       </c>
       <c r="B19" s="18"/>
-      <c r="C19" s="15"/>
+      <c r="C19" s="18"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -2907,7 +2915,7 @@
         <v>0.385416666666667</v>
       </c>
       <c r="B20" s="18"/>
-      <c r="C20" s="16"/>
+      <c r="C20" s="18"/>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
@@ -2920,7 +2928,7 @@
         <v>0.395833333333334</v>
       </c>
       <c r="B21" s="18"/>
-      <c r="C21" s="15"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -2945,8 +2953,8 @@
         <f>A22+TIME(0,myinterval,0)</f>
         <v>0.416666666666667</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>25</v>
+      <c r="B23" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -2960,8 +2968,10 @@
         <f>A23+TIME(0,myinterval,0)</f>
         <v>0.427083333333334</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="16"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
@@ -2973,8 +2983,8 @@
         <f>A24+TIME(0,myinterval,0)</f>
         <v>0.4375</v>
       </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="15"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -2986,8 +2996,8 @@
         <f>A25+TIME(0,myinterval,0)</f>
         <v>0.447916666666667</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="16"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="23"/>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
@@ -2999,8 +3009,8 @@
         <f>A26+TIME(0,myinterval,0)</f>
         <v>0.458333333333334</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="15"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="23"/>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -3012,10 +3022,10 @@
         <f>A27+TIME(0,myinterval,0)</f>
         <v>0.46875</v>
       </c>
-      <c r="B28" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="16"/>
+      <c r="B28" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="23"/>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
@@ -3027,8 +3037,8 @@
         <f>A28+TIME(0,myinterval,0)</f>
         <v>0.479166666666667</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="15"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="23"/>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -3041,9 +3051,9 @@
         <v>0.489583333333334</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="16"/>
+        <v>29</v>
+      </c>
+      <c r="C30" s="23"/>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
@@ -3056,7 +3066,7 @@
         <v>0.5</v>
       </c>
       <c r="B31" s="18"/>
-      <c r="C31" s="15"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
@@ -3081,7 +3091,7 @@
         <f>A32+TIME(0,myinterval,0)</f>
         <v>0.520833333333334</v>
       </c>
-      <c r="B33" s="22"/>
+      <c r="B33" s="19"/>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
@@ -3133,7 +3143,7 @@
         <v>0.5625</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
@@ -3186,7 +3196,7 @@
         <f>A40+TIME(0,myinterval,0)</f>
         <v>0.604166666666667</v>
       </c>
-      <c r="B41" s="22"/>
+      <c r="B41" s="19"/>
       <c r="C41" s="15"/>
       <c r="D41" s="15"/>
       <c r="E41" s="15"/>
@@ -3213,7 +3223,7 @@
         <v>0.625</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C43" s="15"/>
       <c r="D43" s="15"/>
@@ -3253,7 +3263,7 @@
         <f>A45+TIME(0,myinterval,0)</f>
         <v>0.65625</v>
       </c>
-      <c r="B46" s="22"/>
+      <c r="B46" s="19"/>
       <c r="C46" s="16"/>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
@@ -3279,8 +3289,8 @@
         <f>A47+TIME(0,myinterval,0)</f>
         <v>0.677083333333333</v>
       </c>
-      <c r="B48" s="23" t="s">
-        <v>27</v>
+      <c r="B48" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -3294,7 +3304,7 @@
         <f>A48+TIME(0,myinterval,0)</f>
         <v>0.6875</v>
       </c>
-      <c r="B49" s="24"/>
+      <c r="B49" s="18"/>
       <c r="C49" s="15"/>
       <c r="D49" s="15"/>
       <c r="E49" s="15"/>
@@ -3307,7 +3317,7 @@
         <f>A49+TIME(0,myinterval,0)</f>
         <v>0.697916666666666</v>
       </c>
-      <c r="B50" s="24"/>
+      <c r="B50" s="18"/>
       <c r="C50" s="16"/>
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
@@ -3320,7 +3330,7 @@
         <f>A50+TIME(0,myinterval,0)</f>
         <v>0.708333333333333</v>
       </c>
-      <c r="B51" s="24"/>
+      <c r="B51" s="18"/>
       <c r="C51" s="15"/>
       <c r="D51" s="15"/>
       <c r="E51" s="15"/>
@@ -3333,7 +3343,7 @@
         <f>A51+TIME(0,myinterval,0)</f>
         <v>0.71875</v>
       </c>
-      <c r="B52" s="24"/>
+      <c r="B52" s="18"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
@@ -3346,7 +3356,7 @@
         <f>A52+TIME(0,myinterval,0)</f>
         <v>0.729166666666666</v>
       </c>
-      <c r="B53" s="25"/>
+      <c r="B53" s="19"/>
       <c r="C53" s="15"/>
       <c r="D53" s="15"/>
       <c r="E53" s="15"/>
@@ -3643,7 +3653,7 @@
     <row r="76" customFormat="true" ht="21" customHeight="true"/>
     <row r="77" customFormat="true" ht="21" customHeight="true" spans="1:2">
       <c r="A77" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B77" s="31">
         <f>26*15</f>
@@ -3661,7 +3671,7 @@
       <c r="B80" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B15:B21"/>
     <mergeCell ref="B23:B27"/>
@@ -3670,6 +3680,8 @@
     <mergeCell ref="B37:B41"/>
     <mergeCell ref="B43:B46"/>
     <mergeCell ref="B48:B53"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="C24:C31"/>
     <mergeCell ref="A7:C8"/>
   </mergeCells>
   <dataValidations count="2">

</xml_diff>

<commit_message>
notes for paging paper
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -2676,8 +2676,8 @@
   <sheetPr/>
   <dimension ref="A2:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -3066,7 +3066,7 @@
         <v>0.5</v>
       </c>
       <c r="B31" s="18"/>
-      <c r="C31" s="25"/>
+      <c r="C31" s="23"/>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
@@ -3079,7 +3079,7 @@
         <v>0.510416666666667</v>
       </c>
       <c r="B32" s="18"/>
-      <c r="C32" s="16"/>
+      <c r="C32" s="23"/>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
@@ -3092,7 +3092,7 @@
         <v>0.520833333333334</v>
       </c>
       <c r="B33" s="19"/>
-      <c r="C33" s="15"/>
+      <c r="C33" s="25"/>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
       <c r="F33" s="15"/>
@@ -3651,7 +3651,7 @@
       <c r="H75" s="15"/>
     </row>
     <row r="76" customFormat="true" ht="21" customHeight="true"/>
-    <row r="77" customFormat="true" ht="21" customHeight="true" spans="1:2">
+    <row r="77" customFormat="true" ht="21" customHeight="true" spans="1:3">
       <c r="A77" t="s">
         <v>30</v>
       </c>
@@ -3659,11 +3659,19 @@
         <f>26*15</f>
         <v>390</v>
       </c>
-    </row>
-    <row r="78" customFormat="true" ht="21" customHeight="true" spans="2:2">
+      <c r="C77">
+        <f>15*15</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="78" customFormat="true" ht="21" customHeight="true" spans="2:3">
       <c r="B78" s="32" t="str">
         <f>IF(AND(B77&lt;0,B77&gt;-60),CONCATENATE("-",QUOTIENT(B77,60),":",TEXT(MOD(ABS(B77),60),"00")),CONCATENATE(QUOTIENT(B77,60),":",TEXT(MOD(ABS(B77),60),"00"),"h"))</f>
         <v>6:30h</v>
+      </c>
+      <c r="C78" s="32" t="str">
+        <f>IF(AND(C77&lt;0,C77&gt;-60),CONCATENATE("-",QUOTIENT(C77,60),":",TEXT(MOD(ABS(C77),60),"00")),CONCATENATE(QUOTIENT(C77,60),":",TEXT(MOD(ABS(C77),60),"00"),"h"))</f>
+        <v>3:45h</v>
       </c>
     </row>
     <row r="79" customFormat="true" ht="21" customHeight="true"/>
@@ -3681,7 +3689,7 @@
     <mergeCell ref="B43:B46"/>
     <mergeCell ref="B48:B53"/>
     <mergeCell ref="C17:C21"/>
-    <mergeCell ref="C24:C31"/>
+    <mergeCell ref="C24:C33"/>
     <mergeCell ref="A7:C8"/>
   </mergeCells>
   <dataValidations count="2">

</xml_diff>

<commit_message>
update notes and timelog
</commit_message>
<xml_diff>
--- a/time-log.xlsx
+++ b/time-log.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="20850" tabRatio="500" activeTab="2"/>
+    <workbookView windowWidth="22560" windowHeight="17250" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data Settings" sheetId="2" r:id="rId1"/>
     <sheet name="Template" sheetId="4" r:id="rId2"/>
     <sheet name="week1" sheetId="3" r:id="rId3"/>
+    <sheet name="week2" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Interval">#REF!</definedName>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
   <si>
     <t>SCHEDULE START TIME</t>
   </si>
@@ -104,6 +105,9 @@
     <t>Finish theos thesis</t>
   </si>
   <si>
+    <t>Branch Shadowing paper 17</t>
+  </si>
+  <si>
     <t>setup new printer for papers</t>
   </si>
   <si>
@@ -119,13 +123,28 @@
     <t>2nd cache paper</t>
   </si>
   <si>
+    <t>update ML questions</t>
+  </si>
+  <si>
     <t>re read paging 15 paper and make notes</t>
+  </si>
+  <si>
+    <t>Weekly meeting</t>
   </si>
   <si>
     <t>finish paging 15 and repeat cache attacks 17 for notes</t>
   </si>
   <si>
+    <t>update notes</t>
+  </si>
+  <si>
+    <t>Branch shadowing paper 17</t>
+  </si>
+  <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>finish read branch shadowing 17</t>
   </si>
 </sst>
 </file>
@@ -136,9 +155,9 @@
     <numFmt numFmtId="176" formatCode="h:mm\ AM/PM"/>
     <numFmt numFmtId="177" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="178" formatCode="[$-409]h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="31">
@@ -226,24 +245,22 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Century Gothic"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Century Gothic"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Century Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Century Gothic"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,13 +274,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Century Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -274,9 +284,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Century Gothic"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -303,9 +313,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="3"/>
+      <name val="Century Gothic"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Century Gothic"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -318,9 +335,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Century Gothic"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -328,6 +345,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Century Gothic"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Century Gothic"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Century Gothic"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -348,20 +381,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Century Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Century Gothic"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,7 +389,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="46">
+  <fills count="47">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,7 +398,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.8"/>
+        <fgColor theme="6" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,7 +446,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.8"/>
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,7 +464,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.249977111117893"/>
+        <fgColor theme="3" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,6 +482,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -469,7 +506,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,13 +518,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -505,31 +548,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,7 +572,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -559,13 +614,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,43 +632,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -625,19 +656,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,6 +759,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -753,7 +787,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -805,24 +848,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -834,150 +859,150 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="41" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="45" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="40" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="46" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="39" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="42" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="44" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="39" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="42" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="40" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="44" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="45" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="43" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="41" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="43" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="15" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="12" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="14" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="11" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="13" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="10" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="12" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="12" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="10" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="9" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
@@ -1023,31 +1048,13 @@
     <xf numFmtId="178" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="10" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="178" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="10" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="178" fontId="7" fillId="2" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="10" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="11" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="11" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="11" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="10" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="10" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="10" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="178" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
@@ -1059,11 +1066,36 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="12" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="177" fontId="6" fillId="10" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="178" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="2" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="12" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="12" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="12" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="13" borderId="4" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="13" borderId="6" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -1074,15 +1106,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
@@ -1428,271 +1459,271 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="2.85833333333333" customWidth="true"/>
-    <col min="2" max="2" width="14.425" style="35" customWidth="true"/>
+    <col min="2" max="2" width="14.425" style="37" customWidth="true"/>
     <col min="3" max="3" width="3.28333333333333" customWidth="true"/>
     <col min="5" max="5" width="2.425" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="36"/>
-      <c r="B1" s="37"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="A1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" ht="38" customHeight="true" spans="1:5">
-      <c r="A2" s="36"/>
-      <c r="B2" s="38" t="s">
+      <c r="A2" s="38"/>
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="38" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="36"/>
+      <c r="E2" s="38"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="36"/>
-      <c r="B3" s="39">
+      <c r="A3" s="38"/>
+      <c r="B3" s="41">
         <v>0.25</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="39" t="s">
+      <c r="C3" s="38"/>
+      <c r="D3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="36"/>
+      <c r="E3" s="38"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="36"/>
-      <c r="B4" s="39">
+      <c r="A4" s="38"/>
+      <c r="B4" s="41">
         <v>0.291666666666667</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="39" t="s">
+      <c r="C4" s="38"/>
+      <c r="D4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="36"/>
+      <c r="E4" s="38"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="36"/>
-      <c r="B5" s="39">
+      <c r="A5" s="38"/>
+      <c r="B5" s="41">
         <v>0.333333333333333</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="39" t="s">
+      <c r="C5" s="38"/>
+      <c r="D5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="38"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="36"/>
-      <c r="B6" s="39">
+      <c r="A6" s="38"/>
+      <c r="B6" s="41">
         <v>0.375</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="39" t="s">
+      <c r="C6" s="38"/>
+      <c r="D6" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="36"/>
+      <c r="E6" s="38"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="36"/>
-      <c r="B7" s="39">
+      <c r="A7" s="38"/>
+      <c r="B7" s="41">
         <v>0.416666666666667</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="39" t="s">
+      <c r="C7" s="38"/>
+      <c r="D7" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="36"/>
+      <c r="E7" s="38"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="36"/>
-      <c r="B8" s="39">
+      <c r="A8" s="38"/>
+      <c r="B8" s="41">
         <v>0.458333333333333</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="39" t="s">
+      <c r="C8" s="38"/>
+      <c r="D8" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="36"/>
+      <c r="E8" s="38"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="36"/>
-      <c r="B9" s="39">
+      <c r="A9" s="38"/>
+      <c r="B9" s="41">
         <v>0.5</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="40" t="s">
+      <c r="C9" s="38"/>
+      <c r="D9" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="36"/>
+      <c r="E9" s="38"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="36"/>
-      <c r="B10" s="39">
+      <c r="A10" s="38"/>
+      <c r="B10" s="41">
         <v>0.541666666666667</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="40" t="s">
+      <c r="C10" s="38"/>
+      <c r="D10" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="36"/>
+      <c r="E10" s="38"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="36"/>
-      <c r="B11" s="39">
+      <c r="A11" s="38"/>
+      <c r="B11" s="41">
         <v>0.583333333333333</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="40" t="s">
+      <c r="C11" s="38"/>
+      <c r="D11" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
+      <c r="E11" s="38"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="36"/>
-      <c r="B12" s="39">
+      <c r="A12" s="38"/>
+      <c r="B12" s="41">
         <v>0.625</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="40" t="s">
+      <c r="C12" s="38"/>
+      <c r="D12" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="36"/>
+      <c r="E12" s="38"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="36"/>
-      <c r="B13" s="39">
+      <c r="A13" s="38"/>
+      <c r="B13" s="41">
         <v>0.666666666666667</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="36"/>
-      <c r="B14" s="39">
+      <c r="A14" s="38"/>
+      <c r="B14" s="41">
         <v>0.708333333333333</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="36"/>
-      <c r="B15" s="39">
+      <c r="A15" s="38"/>
+      <c r="B15" s="41">
         <v>0.75</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="36"/>
-      <c r="B16" s="39">
+      <c r="A16" s="38"/>
+      <c r="B16" s="41">
         <v>0.791666666666667</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="36"/>
-      <c r="B17" s="39">
+      <c r="A17" s="38"/>
+      <c r="B17" s="41">
         <v>0.833333333333333</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="36"/>
-      <c r="B18" s="39">
+      <c r="A18" s="38"/>
+      <c r="B18" s="41">
         <v>0.875</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="36"/>
-      <c r="B19" s="39">
+      <c r="A19" s="38"/>
+      <c r="B19" s="41">
         <v>0.916666666666667</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="36"/>
-      <c r="B20" s="39">
+      <c r="A20" s="38"/>
+      <c r="B20" s="41">
         <v>0.958333333333333</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="36"/>
-      <c r="B21" s="39">
+      <c r="A21" s="38"/>
+      <c r="B21" s="41">
         <v>0</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="36"/>
-      <c r="B22" s="39">
+      <c r="A22" s="38"/>
+      <c r="B22" s="41">
         <v>0.0416666666666667</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="36"/>
-      <c r="B23" s="39">
+      <c r="A23" s="38"/>
+      <c r="B23" s="41">
         <v>0.0833333333333333</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="36"/>
-      <c r="B24" s="39">
+      <c r="A24" s="38"/>
+      <c r="B24" s="41">
         <v>0.125</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="36"/>
-      <c r="B25" s="39">
+      <c r="A25" s="38"/>
+      <c r="B25" s="41">
         <v>0.166666666666667</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="36"/>
-      <c r="B26" s="39">
+      <c r="A26" s="38"/>
+      <c r="B26" s="41">
         <v>0.208333333333333</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="36"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1707,7 +1738,7 @@
   <dimension ref="A2:H80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C25" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -1720,7 +1751,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:2">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1747,13 +1778,13 @@
       <c r="D8" s="6">
         <v>0.291666666666667</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="21">
         <v>44319</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="22">
         <f>--LEFT(E8,3)</f>
         <v>15</v>
       </c>
@@ -1777,10 +1808,10 @@
       <c r="F9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="23" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1806,11 +1837,11 @@
         <f t="shared" si="0"/>
         <v>44323</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="24">
         <f t="shared" si="0"/>
         <v>44324</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="24">
         <f t="shared" si="0"/>
         <v>44325</v>
       </c>
@@ -2688,8 +2719,8 @@
   <sheetPr/>
   <dimension ref="A2:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -2702,7 +2733,7 @@
   </cols>
   <sheetData>
     <row r="2" s="1" customFormat="true" spans="2:3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2732,13 +2763,13 @@
       <c r="D8" s="6">
         <v>0.291666666666667</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="21">
         <v>44319</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="22">
         <f>--LEFT(E8,3)</f>
         <v>15</v>
       </c>
@@ -2762,10 +2793,10 @@
       <c r="F9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="23" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2791,11 +2822,11 @@
         <f t="shared" si="0"/>
         <v>44323</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="24">
         <f t="shared" si="0"/>
         <v>44324</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="24">
         <f t="shared" si="0"/>
         <v>44325</v>
       </c>
@@ -2857,11 +2888,11 @@
         <f>A14+TIME(0,myinterval,0)</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="26" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="15"/>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="26" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="15"/>
@@ -2874,9 +2905,9 @@
         <f>A15+TIME(0,myinterval,0)</f>
         <v>0.34375</v>
       </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="16"/>
-      <c r="D16" s="18"/>
+      <c r="D16" s="27"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -2887,11 +2918,11 @@
         <f>A16+TIME(0,myinterval,0)</f>
         <v>0.354166666666667</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="17" t="s">
+      <c r="B17" s="27"/>
+      <c r="C17" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="18"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
@@ -2902,9 +2933,9 @@
         <f>A17+TIME(0,myinterval,0)</f>
         <v>0.364583333333333</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
@@ -2915,10 +2946,12 @@
         <f>A18+TIME(0,myinterval,0)</f>
         <v>0.375</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="15"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="26" t="s">
+        <v>27</v>
+      </c>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
@@ -2928,10 +2961,10 @@
         <f>A19+TIME(0,myinterval,0)</f>
         <v>0.385416666666667</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="16"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
@@ -2941,10 +2974,10 @@
         <f>A20+TIME(0,myinterval,0)</f>
         <v>0.395833333333334</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="15"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="27"/>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
@@ -2957,7 +2990,7 @@
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
+      <c r="E22" s="28"/>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
@@ -2967,11 +3000,11 @@
         <f>A22+TIME(0,myinterval,0)</f>
         <v>0.416666666666667</v>
       </c>
-      <c r="B23" s="20" t="s">
-        <v>27</v>
+      <c r="B23" s="29" t="s">
+        <v>28</v>
       </c>
       <c r="C23" s="15"/>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="26" t="s">
         <v>25</v>
       </c>
       <c r="E23" s="15"/>
@@ -2984,11 +3017,11 @@
         <f>A23+TIME(0,myinterval,0)</f>
         <v>0.427083333333334</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="18"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="27"/>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
@@ -2999,10 +3032,12 @@
         <f>A24+TIME(0,myinterval,0)</f>
         <v>0.4375</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="15"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="26" t="s">
+        <v>27</v>
+      </c>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
@@ -3012,10 +3047,10 @@
         <f>A25+TIME(0,myinterval,0)</f>
         <v>0.447916666666667</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="18"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
+      <c r="E26" s="27"/>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
       <c r="H26" s="16"/>
@@ -3025,10 +3060,10 @@
         <f>A26+TIME(0,myinterval,0)</f>
         <v>0.458333333333334</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="18"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
+      <c r="E27" s="27"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
@@ -3038,14 +3073,14 @@
         <f>A27+TIME(0,myinterval,0)</f>
         <v>0.46875</v>
       </c>
-      <c r="B28" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="17" t="s">
+      <c r="B28" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="27"/>
+      <c r="D28" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="16"/>
+      <c r="E28" s="27"/>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
@@ -3055,10 +3090,10 @@
         <f>A28+TIME(0,myinterval,0)</f>
         <v>0.479166666666667</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="15"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
@@ -3068,12 +3103,12 @@
         <f>A29+TIME(0,myinterval,0)</f>
         <v>0.489583333333334</v>
       </c>
-      <c r="B30" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="16"/>
+      <c r="B30" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
       <c r="H30" s="16"/>
@@ -3083,10 +3118,10 @@
         <f>A30+TIME(0,myinterval,0)</f>
         <v>0.5</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="15"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="27"/>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
@@ -3096,10 +3131,10 @@
         <f>A31+TIME(0,myinterval,0)</f>
         <v>0.510416666666667</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
+      <c r="E32" s="28"/>
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>
       <c r="H32" s="16"/>
@@ -3109,8 +3144,8 @@
         <f>A32+TIME(0,myinterval,0)</f>
         <v>0.520833333333334</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
       <c r="F33" s="15"/>
@@ -3149,8 +3184,8 @@
       </c>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
-      <c r="D36" s="23" t="s">
-        <v>31</v>
+      <c r="D36" s="26" t="s">
+        <v>32</v>
       </c>
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
@@ -3162,12 +3197,14 @@
         <f>A36+TIME(0,myinterval,0)</f>
         <v>0.5625</v>
       </c>
-      <c r="B37" s="17" t="s">
-        <v>30</v>
+      <c r="B37" s="26" t="s">
+        <v>31</v>
       </c>
       <c r="C37" s="15"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="15"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="26" t="s">
+        <v>33</v>
+      </c>
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
@@ -3177,12 +3214,12 @@
         <f>A37+TIME(0,myinterval,0)</f>
         <v>0.572916666666667</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D38" s="24"/>
-      <c r="E38" s="16"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
       <c r="H38" s="16"/>
@@ -3192,10 +3229,10 @@
         <f>A38+TIME(0,myinterval,0)</f>
         <v>0.583333333333333</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="15"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
       <c r="F39" s="15"/>
       <c r="G39" s="15"/>
       <c r="H39" s="15"/>
@@ -3205,10 +3242,10 @@
         <f>A39+TIME(0,myinterval,0)</f>
         <v>0.59375</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="16"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
       <c r="F40" s="16"/>
       <c r="G40" s="16"/>
       <c r="H40" s="16"/>
@@ -3218,10 +3255,10 @@
         <f>A40+TIME(0,myinterval,0)</f>
         <v>0.604166666666667</v>
       </c>
-      <c r="B41" s="19"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="15"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="28"/>
       <c r="F41" s="15"/>
       <c r="G41" s="15"/>
       <c r="H41" s="15"/>
@@ -3232,8 +3269,8 @@
         <v>0.614583333333333</v>
       </c>
       <c r="B42" s="16"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="24"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="27"/>
       <c r="E42" s="16"/>
       <c r="F42" s="16"/>
       <c r="G42" s="16"/>
@@ -3244,12 +3281,14 @@
         <f>A42+TIME(0,myinterval,0)</f>
         <v>0.625</v>
       </c>
-      <c r="B43" s="17" t="s">
-        <v>30</v>
+      <c r="B43" s="26" t="s">
+        <v>31</v>
       </c>
       <c r="C43" s="15"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="15"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="32" t="s">
+        <v>35</v>
+      </c>
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
       <c r="H43" s="15"/>
@@ -3259,10 +3298,10 @@
         <f>A43+TIME(0,myinterval,0)</f>
         <v>0.635416666666667</v>
       </c>
-      <c r="B44" s="18"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="16"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="16"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="33"/>
       <c r="F44" s="16"/>
       <c r="G44" s="16"/>
       <c r="H44" s="16"/>
@@ -3272,12 +3311,14 @@
         <f>A44+TIME(0,myinterval,0)</f>
         <v>0.645833333333333</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D45" s="24"/>
-      <c r="E45" s="15"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D45" s="27"/>
+      <c r="E45" s="26" t="s">
+        <v>37</v>
+      </c>
       <c r="F45" s="15"/>
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
@@ -3287,10 +3328,10 @@
         <f>A45+TIME(0,myinterval,0)</f>
         <v>0.65625</v>
       </c>
-      <c r="B46" s="19"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="16"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="28"/>
       <c r="F46" s="16"/>
       <c r="G46" s="16"/>
       <c r="H46" s="16"/>
@@ -3301,8 +3342,8 @@
         <v>0.666666666666666</v>
       </c>
       <c r="B47" s="15"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="25"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="28"/>
       <c r="E47" s="15"/>
       <c r="F47" s="15"/>
       <c r="G47" s="15"/>
@@ -3313,10 +3354,10 @@
         <f>A47+TIME(0,myinterval,0)</f>
         <v>0.677083333333333</v>
       </c>
-      <c r="B48" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C48" s="18"/>
+      <c r="B48" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="27"/>
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
       <c r="F48" s="16"/>
@@ -3328,10 +3369,12 @@
         <f>A48+TIME(0,myinterval,0)</f>
         <v>0.6875</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="19"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="28"/>
       <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
+      <c r="E49" s="26" t="s">
+        <v>38</v>
+      </c>
       <c r="F49" s="15"/>
       <c r="G49" s="15"/>
       <c r="H49" s="15"/>
@@ -3341,10 +3384,10 @@
         <f>A49+TIME(0,myinterval,0)</f>
         <v>0.697916666666666</v>
       </c>
-      <c r="B50" s="18"/>
+      <c r="B50" s="27"/>
       <c r="C50" s="16"/>
       <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
+      <c r="E50" s="27"/>
       <c r="F50" s="16"/>
       <c r="G50" s="16"/>
       <c r="H50" s="16"/>
@@ -3354,10 +3397,10 @@
         <f>A50+TIME(0,myinterval,0)</f>
         <v>0.708333333333333</v>
       </c>
-      <c r="B51" s="18"/>
+      <c r="B51" s="27"/>
       <c r="C51" s="15"/>
       <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
+      <c r="E51" s="28"/>
       <c r="F51" s="15"/>
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
@@ -3367,7 +3410,7 @@
         <f>A51+TIME(0,myinterval,0)</f>
         <v>0.71875</v>
       </c>
-      <c r="B52" s="18"/>
+      <c r="B52" s="27"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
@@ -3380,7 +3423,7 @@
         <f>A52+TIME(0,myinterval,0)</f>
         <v>0.729166666666666</v>
       </c>
-      <c r="B53" s="19"/>
+      <c r="B53" s="28"/>
       <c r="C53" s="15"/>
       <c r="D53" s="15"/>
       <c r="E53" s="15"/>
@@ -3675,11 +3718,11 @@
       <c r="H75" s="15"/>
     </row>
     <row r="76" customFormat="true" ht="21" customHeight="true"/>
-    <row r="77" customFormat="true" ht="21" customHeight="true" spans="1:4">
+    <row r="77" customFormat="true" ht="21" customHeight="true" spans="1:5">
       <c r="A77" t="s">
-        <v>34</v>
-      </c>
-      <c r="B77" s="31">
+        <v>39</v>
+      </c>
+      <c r="B77" s="34">
         <f>26*15</f>
         <v>390</v>
       </c>
@@ -3691,27 +3734,35 @@
         <f>26*15</f>
         <v>390</v>
       </c>
-    </row>
-    <row r="78" customFormat="true" ht="21" customHeight="true" spans="2:4">
-      <c r="B78" s="32" t="str">
+      <c r="E77">
+        <f>24*15</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="78" customFormat="true" ht="21" customHeight="true" spans="2:5">
+      <c r="B78" s="35" t="str">
         <f>IF(AND(B77&lt;0,B77&gt;-60),CONCATENATE("-",QUOTIENT(B77,60),":",TEXT(MOD(ABS(B77),60),"00")),CONCATENATE(QUOTIENT(B77,60),":",TEXT(MOD(ABS(B77),60),"00"),"h"))</f>
         <v>6:30h</v>
       </c>
-      <c r="C78" s="32" t="str">
+      <c r="C78" s="35" t="str">
         <f>IF(AND(C77&lt;0,C77&gt;-60),CONCATENATE("-",QUOTIENT(C77,60),":",TEXT(MOD(ABS(C77),60),"00")),CONCATENATE(QUOTIENT(C77,60),":",TEXT(MOD(ABS(C77),60),"00"),"h"))</f>
         <v>6:15h</v>
       </c>
-      <c r="D78" s="32" t="str">
+      <c r="D78" s="35" t="str">
         <f>IF(AND(D77&lt;0,D77&gt;-60),CONCATENATE("-",QUOTIENT(D77,60),":",TEXT(MOD(ABS(D77),60),"00")),CONCATENATE(QUOTIENT(D77,60),":",TEXT(MOD(ABS(D77),60),"00"),"h"))</f>
         <v>6:30h</v>
       </c>
+      <c r="E78" s="35" t="str">
+        <f>IF(AND(E77&lt;0,E77&gt;-60),CONCATENATE("-",QUOTIENT(E77,60),":",TEXT(MOD(ABS(E77),60),"00")),CONCATENATE(QUOTIENT(E77,60),":",TEXT(MOD(ABS(E77),60),"00"),"h"))</f>
+        <v>6:00h</v>
+      </c>
     </row>
     <row r="79" customFormat="true" ht="21" customHeight="true"/>
     <row r="80" customFormat="true" ht="21" customHeight="true" spans="2:2">
-      <c r="B80" s="33"/>
+      <c r="B80" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="23">
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B15:B21"/>
     <mergeCell ref="B23:B27"/>
@@ -3728,6 +3779,997 @@
     <mergeCell ref="D23:D25"/>
     <mergeCell ref="D28:D31"/>
     <mergeCell ref="D36:D47"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="E25:E32"/>
+    <mergeCell ref="E37:E41"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="A7:C8"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8">
+      <formula1>'Data Settings'!$D$3:$D$12</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8">
+      <formula1>'Data Settings'!$B$3:$B$26</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A2:H80"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="14.5" style="1" customWidth="true"/>
+    <col min="2" max="8" width="21.5" style="1" customWidth="true"/>
+    <col min="9" max="9" width="10.7083333333333" style="1"/>
+    <col min="10" max="10" width="12.625" style="1"/>
+    <col min="11" max="16384" width="10.7083333333333" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" s="1" customFormat="true" spans="2:2">
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="true" ht="18" customHeight="true" spans="1:6">
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="true" ht="20" customHeight="true" spans="1:7">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="6">
+        <v>0.291666666666667</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="21">
+        <v>44319</v>
+      </c>
+      <c r="G8" s="22">
+        <f>--LEFT(E8,3)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="true" ht="18" customHeight="true" spans="1:8">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12">
+        <f>F8</f>
+        <v>44319</v>
+      </c>
+      <c r="C10" s="13">
+        <f t="shared" ref="C10:H10" si="0">B10+1</f>
+        <v>44320</v>
+      </c>
+      <c r="D10" s="14">
+        <f t="shared" si="0"/>
+        <v>44321</v>
+      </c>
+      <c r="E10" s="13">
+        <f t="shared" si="0"/>
+        <v>44322</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="0"/>
+        <v>44323</v>
+      </c>
+      <c r="G10" s="24">
+        <f t="shared" si="0"/>
+        <v>44324</v>
+      </c>
+      <c r="H10" s="24">
+        <f t="shared" si="0"/>
+        <v>44325</v>
+      </c>
+    </row>
+    <row r="11" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A11" s="15">
+        <f>D8</f>
+        <v>0.291666666666667</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A12" s="16">
+        <f>A11+TIME(0,myinterval,0)</f>
+        <v>0.302083333333334</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A13" s="15">
+        <f>A12+TIME(0,myinterval,0)</f>
+        <v>0.3125</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A14" s="16">
+        <f>A13+TIME(0,myinterval,0)</f>
+        <v>0.322916666666667</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A15" s="15">
+        <f>A14+TIME(0,myinterval,0)</f>
+        <v>0.333333333333334</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A16" s="16">
+        <f>A15+TIME(0,myinterval,0)</f>
+        <v>0.34375</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+    </row>
+    <row r="17" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A17" s="15">
+        <f>A16+TIME(0,myinterval,0)</f>
+        <v>0.354166666666667</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A18" s="16">
+        <f>A17+TIME(0,myinterval,0)</f>
+        <v>0.364583333333334</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A19" s="15">
+        <f>A18+TIME(0,myinterval,0)</f>
+        <v>0.375</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+    </row>
+    <row r="20" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A20" s="16">
+        <f>A19+TIME(0,myinterval,0)</f>
+        <v>0.385416666666667</v>
+      </c>
+      <c r="B20" s="18"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+    </row>
+    <row r="21" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A21" s="15">
+        <f>A20+TIME(0,myinterval,0)</f>
+        <v>0.395833333333334</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A22" s="16">
+        <f>A21+TIME(0,myinterval,0)</f>
+        <v>0.406250000000001</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+    </row>
+    <row r="23" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A23" s="15">
+        <f>A22+TIME(0,myinterval,0)</f>
+        <v>0.416666666666667</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+    </row>
+    <row r="24" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A24" s="16">
+        <f>A23+TIME(0,myinterval,0)</f>
+        <v>0.427083333333334</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+    </row>
+    <row r="25" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A25" s="15">
+        <f>A24+TIME(0,myinterval,0)</f>
+        <v>0.437500000000001</v>
+      </c>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+    </row>
+    <row r="26" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A26" s="16">
+        <f>A25+TIME(0,myinterval,0)</f>
+        <v>0.447916666666667</v>
+      </c>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+    </row>
+    <row r="27" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A27" s="15">
+        <f>A26+TIME(0,myinterval,0)</f>
+        <v>0.458333333333334</v>
+      </c>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A28" s="16">
+        <f>A27+TIME(0,myinterval,0)</f>
+        <v>0.468750000000001</v>
+      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+    </row>
+    <row r="29" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A29" s="15">
+        <f>A28+TIME(0,myinterval,0)</f>
+        <v>0.479166666666667</v>
+      </c>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+    </row>
+    <row r="30" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A30" s="16">
+        <f>A29+TIME(0,myinterval,0)</f>
+        <v>0.489583333333334</v>
+      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+    </row>
+    <row r="31" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A31" s="15">
+        <f>A30+TIME(0,myinterval,0)</f>
+        <v>0.500000000000001</v>
+      </c>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+    </row>
+    <row r="32" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A32" s="16">
+        <f>A31+TIME(0,myinterval,0)</f>
+        <v>0.510416666666667</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+    </row>
+    <row r="33" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A33" s="15">
+        <f>A32+TIME(0,myinterval,0)</f>
+        <v>0.520833333333334</v>
+      </c>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+    </row>
+    <row r="34" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A34" s="16">
+        <f>A33+TIME(0,myinterval,0)</f>
+        <v>0.531250000000001</v>
+      </c>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+    </row>
+    <row r="35" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A35" s="15">
+        <f>A34+TIME(0,myinterval,0)</f>
+        <v>0.541666666666667</v>
+      </c>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+    </row>
+    <row r="36" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A36" s="16">
+        <f>A35+TIME(0,myinterval,0)</f>
+        <v>0.552083333333334</v>
+      </c>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+    </row>
+    <row r="37" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A37" s="15">
+        <f>A36+TIME(0,myinterval,0)</f>
+        <v>0.5625</v>
+      </c>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+    </row>
+    <row r="38" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A38" s="16">
+        <f>A37+TIME(0,myinterval,0)</f>
+        <v>0.572916666666667</v>
+      </c>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+    </row>
+    <row r="39" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A39" s="15">
+        <f>A38+TIME(0,myinterval,0)</f>
+        <v>0.583333333333334</v>
+      </c>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+    </row>
+    <row r="40" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A40" s="16">
+        <f>A39+TIME(0,myinterval,0)</f>
+        <v>0.59375</v>
+      </c>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+    </row>
+    <row r="41" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A41" s="15">
+        <f>A40+TIME(0,myinterval,0)</f>
+        <v>0.604166666666667</v>
+      </c>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+    </row>
+    <row r="42" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A42" s="16">
+        <f>A41+TIME(0,myinterval,0)</f>
+        <v>0.614583333333334</v>
+      </c>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+    </row>
+    <row r="43" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A43" s="15">
+        <f>A42+TIME(0,myinterval,0)</f>
+        <v>0.625</v>
+      </c>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+    </row>
+    <row r="44" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A44" s="16">
+        <f>A43+TIME(0,myinterval,0)</f>
+        <v>0.635416666666667</v>
+      </c>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+    </row>
+    <row r="45" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A45" s="15">
+        <f>A44+TIME(0,myinterval,0)</f>
+        <v>0.645833333333333</v>
+      </c>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+    </row>
+    <row r="46" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A46" s="16">
+        <f>A45+TIME(0,myinterval,0)</f>
+        <v>0.65625</v>
+      </c>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+    </row>
+    <row r="47" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A47" s="15">
+        <f>A46+TIME(0,myinterval,0)</f>
+        <v>0.666666666666667</v>
+      </c>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+    </row>
+    <row r="48" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A48" s="16">
+        <f>A47+TIME(0,myinterval,0)</f>
+        <v>0.677083333333333</v>
+      </c>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+    </row>
+    <row r="49" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A49" s="15">
+        <f>A48+TIME(0,myinterval,0)</f>
+        <v>0.6875</v>
+      </c>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+    </row>
+    <row r="50" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A50" s="16">
+        <f>A49+TIME(0,myinterval,0)</f>
+        <v>0.697916666666667</v>
+      </c>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+    </row>
+    <row r="51" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A51" s="15">
+        <f>A50+TIME(0,myinterval,0)</f>
+        <v>0.708333333333333</v>
+      </c>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+    </row>
+    <row r="52" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A52" s="16">
+        <f>A51+TIME(0,myinterval,0)</f>
+        <v>0.71875</v>
+      </c>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+    </row>
+    <row r="53" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A53" s="15">
+        <f>A52+TIME(0,myinterval,0)</f>
+        <v>0.729166666666667</v>
+      </c>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+    </row>
+    <row r="54" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A54" s="16">
+        <f>A53+TIME(0,myinterval,0)</f>
+        <v>0.739583333333333</v>
+      </c>
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+    </row>
+    <row r="55" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A55" s="15">
+        <f>A54+TIME(0,myinterval,0)</f>
+        <v>0.75</v>
+      </c>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+    </row>
+    <row r="56" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A56" s="16">
+        <f>A55+TIME(0,myinterval,0)</f>
+        <v>0.760416666666666</v>
+      </c>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+    </row>
+    <row r="57" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A57" s="15">
+        <f>A56+TIME(0,myinterval,0)</f>
+        <v>0.770833333333333</v>
+      </c>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+    </row>
+    <row r="58" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A58" s="16">
+        <f>A57+TIME(0,myinterval,0)</f>
+        <v>0.78125</v>
+      </c>
+      <c r="B58" s="16"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+    </row>
+    <row r="59" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A59" s="15">
+        <f>A58+TIME(0,myinterval,0)</f>
+        <v>0.791666666666666</v>
+      </c>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+    </row>
+    <row r="60" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A60" s="16">
+        <f>A59+TIME(0,myinterval,0)</f>
+        <v>0.802083333333333</v>
+      </c>
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="16"/>
+    </row>
+    <row r="61" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A61" s="15">
+        <f>A60+TIME(0,myinterval,0)</f>
+        <v>0.8125</v>
+      </c>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+    </row>
+    <row r="62" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A62" s="16">
+        <f>A61+TIME(0,myinterval,0)</f>
+        <v>0.822916666666666</v>
+      </c>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
+    </row>
+    <row r="63" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A63" s="15">
+        <f>A62+TIME(0,myinterval,0)</f>
+        <v>0.833333333333333</v>
+      </c>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+    </row>
+    <row r="64" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A64" s="16">
+        <f>A63+TIME(0,myinterval,0)</f>
+        <v>0.843749999999999</v>
+      </c>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16"/>
+    </row>
+    <row r="65" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A65" s="15">
+        <f>A64+TIME(0,myinterval,0)</f>
+        <v>0.854166666666666</v>
+      </c>
+      <c r="B65" s="15"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+    </row>
+    <row r="66" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A66" s="16">
+        <f>A65+TIME(0,myinterval,0)</f>
+        <v>0.864583333333333</v>
+      </c>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="16"/>
+    </row>
+    <row r="67" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A67" s="15">
+        <f>A66+TIME(0,myinterval,0)</f>
+        <v>0.874999999999999</v>
+      </c>
+      <c r="B67" s="15"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+    </row>
+    <row r="68" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A68" s="16">
+        <f>A67+TIME(0,myinterval,0)</f>
+        <v>0.885416666666666</v>
+      </c>
+      <c r="B68" s="16"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="16"/>
+    </row>
+    <row r="69" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A69" s="15">
+        <f>A68+TIME(0,myinterval,0)</f>
+        <v>0.895833333333333</v>
+      </c>
+      <c r="B69" s="15"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
+    </row>
+    <row r="70" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A70" s="16">
+        <f>A69+TIME(0,myinterval,0)</f>
+        <v>0.906249999999999</v>
+      </c>
+      <c r="B70" s="16"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
+    </row>
+    <row r="71" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A71" s="15">
+        <f>A70+TIME(0,myinterval,0)</f>
+        <v>0.916666666666666</v>
+      </c>
+      <c r="B71" s="15"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
+    </row>
+    <row r="72" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A72" s="16">
+        <f>A71+TIME(0,myinterval,0)</f>
+        <v>0.927083333333332</v>
+      </c>
+      <c r="B72" s="16"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="16"/>
+      <c r="H72" s="16"/>
+    </row>
+    <row r="73" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A73" s="15">
+        <f>A72+TIME(0,myinterval,0)</f>
+        <v>0.937499999999999</v>
+      </c>
+      <c r="B73" s="15"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
+    </row>
+    <row r="74" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A74" s="16">
+        <f>A73+TIME(0,myinterval,0)</f>
+        <v>0.947916666666666</v>
+      </c>
+      <c r="B74" s="16"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="16"/>
+    </row>
+    <row r="75" s="1" customFormat="true" ht="21" customHeight="true" spans="1:8">
+      <c r="A75" s="15">
+        <f>A74+TIME(0,myinterval,0)</f>
+        <v>0.958333333333332</v>
+      </c>
+      <c r="B75" s="15"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="15"/>
+      <c r="F75" s="15"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="15"/>
+    </row>
+    <row r="76" customFormat="true" ht="21" customHeight="true"/>
+    <row r="77" customFormat="true" ht="21" customHeight="true"/>
+    <row r="78" customFormat="true" ht="21" customHeight="true"/>
+    <row r="79" customFormat="true" ht="21" customHeight="true"/>
+    <row r="80" customFormat="true" ht="21" customHeight="true"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B16:B23"/>
     <mergeCell ref="A7:C8"/>
   </mergeCells>
   <dataValidations count="2">

</xml_diff>